<commit_message>
bits v5 board nearly done
</commit_message>
<xml_diff>
--- a/Boards/BITSv5/BOM.xlsx
+++ b/Boards/BITSv5/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Storage\BPP\Command\command_module\Boards\BITSv5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F598218-BEA7-4C4A-AE44-1A4C78D77B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A60897-0C1D-4E75-86AD-D48985EA7832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="188">
   <si>
     <t>Part ID</t>
   </si>
@@ -555,9 +555,6 @@
     <t>Molex PB</t>
   </si>
   <si>
-    <t>RP2040 Reset</t>
-  </si>
-  <si>
     <t>Memory Boot</t>
   </si>
   <si>
@@ -580,6 +577,18 @@
   </si>
   <si>
     <t>XBP9X-DMUS-001</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/molex/0532611071/699102?s=N4IgTCBcDaILYHsA2BTAHgAgA4EsDGCARkgIYAmKGArAMxgBsAjALSMAMA7IyALoC%2BQA</t>
+  </si>
+  <si>
+    <t>must order connecting piece</t>
+  </si>
+  <si>
+    <t>Power Slider</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nidec-components-corporation/CL-SB-12B-01T/3507823</t>
   </si>
 </sst>
 </file>
@@ -947,11 +956,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -966,7 +975,7 @@
     <col min="8" max="8" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -992,7 +1001,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1018,7 +1027,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1044,7 +1053,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1070,7 +1079,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -1096,7 +1105,7 @@
         <v>2.41</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>27</v>
       </c>
@@ -1122,12 +1131,12 @@
         <v>2.74</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C7" t="s">
         <v>93</v>
@@ -1143,7 +1152,7 @@
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>143</v>
       </c>
@@ -1166,7 +1175,7 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>144</v>
       </c>
@@ -1192,7 +1201,7 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>145</v>
       </c>
@@ -1218,7 +1227,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>146</v>
       </c>
@@ -1238,18 +1247,18 @@
         <v>168</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H11" s="3">
         <v>0.61</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
@@ -1265,7 +1274,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
@@ -1278,8 +1287,17 @@
       <c r="F15" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G15" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1.07</v>
+      </c>
+      <c r="I15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>36</v>
       </c>
@@ -1299,7 +1317,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>37</v>
       </c>
@@ -1319,24 +1337,24 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>162</v>
       </c>
       <c r="B18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" t="s">
         <v>178</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="F18" t="s">
         <v>180</v>
       </c>
-      <c r="F18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>114</v>
       </c>
@@ -1344,15 +1362,21 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C21" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="H21" s="3">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>39</v>
       </c>
@@ -1369,7 +1393,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>40</v>
       </c>
@@ -1386,7 +1410,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>41</v>
       </c>
@@ -1400,7 +1424,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>42</v>
       </c>
@@ -1414,7 +1438,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>43</v>
       </c>
@@ -1425,7 +1449,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>44</v>
       </c>
@@ -1439,7 +1463,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>45</v>
       </c>
@@ -1453,7 +1477,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>46</v>
       </c>
@@ -1467,7 +1491,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>47</v>
       </c>
@@ -1481,7 +1505,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>48</v>
       </c>
@@ -2150,9 +2174,11 @@
     <hyperlink ref="G3" r:id="rId4" xr:uid="{BA500261-FCC6-4C4D-9542-34F3F09F432B}"/>
     <hyperlink ref="G71" r:id="rId5" xr:uid="{47D3ADE3-C448-46ED-ACFD-2A0F339F3E7E}"/>
     <hyperlink ref="G6" r:id="rId6" xr:uid="{96923E9C-BB4B-47C8-9A3C-A7C6B1A96847}"/>
+    <hyperlink ref="G15" r:id="rId7" xr:uid="{782FF733-0012-458C-B7BF-28A0E433F420}"/>
+    <hyperlink ref="G21" r:id="rId8" xr:uid="{19B5DCE6-A05F-4D62-86CA-07D78ADFE698}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId7"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId9"/>
   <ignoredErrors>
     <ignoredError sqref="E38 E43" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
bits v5 board feedback added
</commit_message>
<xml_diff>
--- a/Boards/BITSv5/BOM.xlsx
+++ b/Boards/BITSv5/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Storage\BPP\Command\command_module\Boards\BITSv5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A60897-0C1D-4E75-86AD-D48985EA7832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27299553-FBB1-4DC8-8E7A-5774C7F68D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="189">
   <si>
     <t>Part ID</t>
   </si>
@@ -589,6 +589,9 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/nidec-components-corporation/CL-SB-12B-01T/3507823</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nidec-components-corporation/CAS-120TB/341662</t>
   </si>
 </sst>
 </file>
@@ -960,7 +963,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1360,6 +1363,12 @@
       </c>
       <c r="C20" t="s">
         <v>176</v>
+      </c>
+      <c r="G20" t="s">
+        <v>188</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1.37</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
xbee joint and bits updates
</commit_message>
<xml_diff>
--- a/Boards/BITSv5/BOM.xlsx
+++ b/Boards/BITSv5/BOM.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Storage\BPP\Command\command_module\Boards\BITSv5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A33DFA-82A2-4CD4-B050-0D04CC192489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D0A46B-D535-41EC-88C2-E19066523A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12480" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="193">
   <si>
     <t>Part ID</t>
   </si>
@@ -63,15 +74,6 @@
     <t>GPS</t>
   </si>
   <si>
-    <t>Flash</t>
-  </si>
-  <si>
-    <t>MAX77857</t>
-  </si>
-  <si>
-    <t>Buck-Boost</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -93,27 +95,9 @@
     <t>Package</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/analog-devices-inc-maxim-integrated/MAX77857BEWB/16499288</t>
-  </si>
-  <si>
-    <t>35WLP</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/u-blox/MAX-M10S-00B/15712906</t>
   </si>
   <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>Boost</t>
-  </si>
-  <si>
-    <t>5V</t>
-  </si>
-  <si>
-    <t>3.3V</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/raspberry-pi/SC0914-13/14306010?s=N4IgTCBcDaIE4AcwAYAsyQF0C%2BQ</t>
   </si>
   <si>
@@ -153,9 +137,6 @@
     <t>R5</t>
   </si>
   <si>
-    <t>R6</t>
-  </si>
-  <si>
     <t>R7</t>
   </si>
   <si>
@@ -174,9 +155,6 @@
     <t>R12</t>
   </si>
   <si>
-    <t>R13</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -273,9 +251,6 @@
     <t>100 nF</t>
   </si>
   <si>
-    <t>220 nF</t>
-  </si>
-  <si>
     <t>2.2 uF</t>
   </si>
   <si>
@@ -300,42 +275,18 @@
     <t>GCT4085</t>
   </si>
   <si>
-    <t>22 uF 25V</t>
-  </si>
-  <si>
-    <t>10 uF 25V</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/texas-instruments/TPS61232DRCR/6110563</t>
-  </si>
-  <si>
-    <t>TPS61232DRCR</t>
-  </si>
-  <si>
-    <t>10-VFDFN</t>
-  </si>
-  <si>
     <t>MAX</t>
   </si>
   <si>
-    <t>SW1</t>
-  </si>
-  <si>
     <t>SW2</t>
   </si>
   <si>
     <t>0603</t>
   </si>
   <si>
-    <t>0805</t>
-  </si>
-  <si>
     <t>0402</t>
   </si>
   <si>
-    <t>470 nF 6.3V</t>
-  </si>
-  <si>
     <t>C26</t>
   </si>
   <si>
@@ -363,12 +314,6 @@
     <t>10 nF</t>
   </si>
   <si>
-    <t>8.2 pF</t>
-  </si>
-  <si>
-    <t>47 pF</t>
-  </si>
-  <si>
     <t>10 uF</t>
   </si>
   <si>
@@ -381,24 +326,9 @@
     <t>1K</t>
   </si>
   <si>
-    <t>1M</t>
-  </si>
-  <si>
     <t>5.1K</t>
   </si>
   <si>
-    <t>~50K</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>178K</t>
-  </si>
-  <si>
-    <t>20K</t>
-  </si>
-  <si>
     <t>2520</t>
   </si>
   <si>
@@ -456,18 +386,9 @@
     <t>3-DFN</t>
   </si>
   <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>XBee Headers</t>
-  </si>
-  <si>
     <t>Debugging</t>
   </si>
   <si>
-    <t>6-Pin JST</t>
-  </si>
-  <si>
     <t>USBLC6-2SC6</t>
   </si>
   <si>
@@ -480,15 +401,6 @@
     <t>Memory Boot</t>
   </si>
   <si>
-    <t>RP2040 SWD/SWCLK</t>
-  </si>
-  <si>
-    <t>Emergencies</t>
-  </si>
-  <si>
-    <t>2-Pin JST</t>
-  </si>
-  <si>
     <t>ECS-120-10-36B2-JTN-TR</t>
   </si>
   <si>
@@ -501,9 +413,6 @@
     <t>https://www.digikey.com/en/products/detail/molex/0532611071/699102?s=N4IgTCBcDaILYHsA2BTAHgAgA4EsDGCARkgIYAmKGArAMxgBsAjALSMAMA7IyALoC%2BQA</t>
   </si>
   <si>
-    <t>must order connecting piece</t>
-  </si>
-  <si>
     <t>Power Slider</t>
   </si>
   <si>
@@ -523,6 +432,189 @@
   </si>
   <si>
     <t>252012CDMCDDS-R47MC</t>
+  </si>
+  <si>
+    <t>MAX25255AFDA/VY+</t>
+  </si>
+  <si>
+    <t>Headers</t>
+  </si>
+  <si>
+    <t>Male Pins</t>
+  </si>
+  <si>
+    <t>SW3</t>
+  </si>
+  <si>
+    <t>CAS-120TB</t>
+  </si>
+  <si>
+    <t>CL-SB-12B-01T</t>
+  </si>
+  <si>
+    <t>0.1 uF</t>
+  </si>
+  <si>
+    <t>4.7 uF</t>
+  </si>
+  <si>
+    <t>100 pF</t>
+  </si>
+  <si>
+    <t>C33</t>
+  </si>
+  <si>
+    <t>C34</t>
+  </si>
+  <si>
+    <t>C35</t>
+  </si>
+  <si>
+    <t>C36</t>
+  </si>
+  <si>
+    <t>C37</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/digi/XBP9X-DMUS-001/5972744</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/ecs-inc/ECS-120-10-36B2-JTN-TR/14663300?s=N4IgTCBcDaIKIGEDKBaAjGADO7BmAbAEJgoBSAKgHIrkBKIAugL5A</t>
+  </si>
+  <si>
+    <t>must order connecting pieces</t>
+  </si>
+  <si>
+    <t>AE1</t>
+  </si>
+  <si>
+    <t>1575AT43A0040001E</t>
+  </si>
+  <si>
+    <t>GPS Antenna</t>
+  </si>
+  <si>
+    <t>0.5-1 dB</t>
+  </si>
+  <si>
+    <t>Chip</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/johanson-technology-inc/1575AT43A0040001E/1560674?s=N4IgTCBcDaIOwEYwFoEAY0GZXIHIBEQBdAXyA</t>
+  </si>
+  <si>
+    <t>BT1</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>Flash Memory</t>
+  </si>
+  <si>
+    <t>Dual Buck</t>
+  </si>
+  <si>
+    <t>Iridium</t>
+  </si>
+  <si>
+    <t>10-Pin</t>
+  </si>
+  <si>
+    <t>3.3V, 5V</t>
+  </si>
+  <si>
+    <t>23-WFQFN</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/analog-devices-inc-maxim-integrated/max25255afda-vy/18693435</t>
+  </si>
+  <si>
+    <t>23.7K</t>
+  </si>
+  <si>
+    <t>5K</t>
+  </si>
+  <si>
+    <t>46.4K</t>
+  </si>
+  <si>
+    <t>510K</t>
+  </si>
+  <si>
+    <t>Transistor</t>
+  </si>
+  <si>
+    <t>PNP</t>
+  </si>
+  <si>
+    <t>NPN</t>
+  </si>
+  <si>
+    <t>SOT23-3</t>
+  </si>
+  <si>
+    <t>SOT23</t>
+  </si>
+  <si>
+    <t>1.5M</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>XT30PW-M</t>
+  </si>
+  <si>
+    <t>Battery Connector</t>
+  </si>
+  <si>
+    <t>XT30</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/gct/USB4085-GF-A/9859662</t>
   </si>
 </sst>
 </file>
@@ -890,11 +982,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C81" sqref="C81"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -903,12 +995,12 @@
     <col min="2" max="2" width="27.26953125" customWidth="1"/>
     <col min="3" max="3" width="18.1796875" customWidth="1"/>
     <col min="4" max="4" width="10.6328125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="11"/>
+    <col min="5" max="5" width="9.6328125" style="11" customWidth="1"/>
     <col min="6" max="6" width="13.6328125" customWidth="1"/>
     <col min="7" max="7" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -919,19 +1011,19 @@
         <v>8</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -942,19 +1034,19 @@
         <v>9</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="G2" s="3">
         <v>0.7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -962,22 +1054,22 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G3" s="3">
         <v>1.68</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -988,987 +1080,1262 @@
         <v>11</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>171</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>28</v>
+        <v>174</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>22</v>
+        <v>176</v>
       </c>
       <c r="G5" s="3">
         <v>2.41</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="3">
+        <v>112.59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2.31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C13" t="s">
+        <v>190</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" t="s">
+        <v>152</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1.07</v>
+      </c>
+      <c r="H17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" t="s">
+        <v>125</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24" t="s">
+        <v>181</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" t="s">
+        <v>181</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="8">
+        <v>27</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="8">
+        <v>27</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="11" t="s">
+      <c r="E29" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G6" s="3">
-        <v>2.74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" t="s">
-        <v>156</v>
-      </c>
-      <c r="C7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G8" s="3">
-        <v>2.31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" t="s">
-        <v>136</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G9" s="3">
-        <v>3.05</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" t="s">
-        <v>131</v>
-      </c>
-      <c r="C10" t="s">
-        <v>132</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" t="s">
-        <v>147</v>
-      </c>
-      <c r="C11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0.61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>154</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+      <c r="E30" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="G15" s="3">
-        <v>1.07</v>
-      </c>
-      <c r="H15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" t="s">
-        <v>144</v>
-      </c>
-      <c r="C17" t="s">
-        <v>145</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B18" t="s">
-        <v>151</v>
-      </c>
-      <c r="C18" t="s">
-        <v>152</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" t="s">
-        <v>150</v>
-      </c>
-      <c r="F20" t="s">
-        <v>161</v>
-      </c>
-      <c r="G20" s="3">
-        <v>1.37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" t="s">
-        <v>159</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="G21" s="3">
-        <v>1.26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" s="8">
-        <v>27</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="8">
-        <v>27</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" t="s">
-        <v>77</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" t="s">
-        <v>77</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" t="s">
-        <v>77</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="8">
-        <v>270</v>
+        <v>66</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="8">
+        <v>470</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
-        <v>50</v>
+        <v>160</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
-        <v>51</v>
+        <v>161</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>80</v>
+        <v>178</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
-        <v>52</v>
+        <v>162</v>
       </c>
       <c r="C40" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>81</v>
+        <v>179</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
-        <v>53</v>
+        <v>163</v>
       </c>
       <c r="C41" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>81</v>
+        <v>186</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
-        <v>54</v>
+        <v>164</v>
       </c>
       <c r="C42" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>81</v>
+        <v>187</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
-        <v>55</v>
+        <v>165</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>81</v>
+        <v>180</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
-        <v>56</v>
+        <v>166</v>
       </c>
       <c r="C44" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="6" t="s">
-        <v>57</v>
+        <v>167</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>81</v>
+        <v>177</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
-        <v>58</v>
+        <v>168</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>81</v>
+        <v>178</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
-        <v>59</v>
+        <v>169</v>
       </c>
       <c r="C47" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C48" t="s">
-        <v>78</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="C50" t="s">
-        <v>78</v>
+        <v>67</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C51" t="s">
-        <v>78</v>
+        <v>67</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="C52" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D52" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E52" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="C53" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D53" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="C54" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C56" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="6" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="C57" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C58" t="s">
-        <v>78</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>92</v>
-      </c>
       <c r="E58" s="11" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="6" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="C59" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="6" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="C60" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="C61" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="6" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="C62" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="6" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="C63" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="6" t="s">
-        <v>104</v>
+        <v>54</v>
       </c>
       <c r="C64" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="6" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C65" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="6" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="C66" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="C67" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="C68" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="6" t="s">
-        <v>109</v>
+        <v>59</v>
       </c>
       <c r="C69" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C70" t="s">
+        <v>67</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B71" t="s">
-        <v>165</v>
+        <v>61</v>
       </c>
       <c r="C71" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="F71" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G71" s="3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C72" t="s">
+        <v>67</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E72" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C73" t="s">
+        <v>67</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E73" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C74" t="s">
+        <v>67</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C75" t="s">
+        <v>67</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C76" t="s">
+        <v>67</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C77" t="s">
+        <v>67</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E77" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C78" t="s">
+        <v>67</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C79" t="s">
+        <v>67</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C80" t="s">
+        <v>67</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E80" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C81" t="s">
+        <v>67</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E81" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C82" t="s">
+        <v>67</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E82" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C83" t="s">
+        <v>67</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E83" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C84" t="s">
+        <v>67</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C85" t="s">
+        <v>67</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B87" t="s">
+        <v>131</v>
+      </c>
+      <c r="C87" t="s">
+        <v>68</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G87" s="3">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A72" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B72" t="s">
-        <v>165</v>
-      </c>
-      <c r="C72" t="s">
-        <v>79</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="E72" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="F72" t="s">
-        <v>164</v>
-      </c>
-      <c r="G72" s="3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B88" t="s">
+        <v>131</v>
+      </c>
+      <c r="C88" t="s">
+        <v>68</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E88" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F88" t="s">
+        <v>130</v>
+      </c>
+      <c r="G88" s="3">
         <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F90" t="s">
+        <v>146</v>
+      </c>
+      <c r="G90" s="3">
+        <f>SUM(G2:G88)</f>
+        <v>152.05000000000001</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" xr:uid="{64199562-BB3C-4F77-8D16-F1B55B1EF228}"/>
-    <hyperlink ref="F4" r:id="rId2" xr:uid="{A178FAE8-B11F-43AB-8C77-7A0C5EC5F6F0}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{390A1AD8-E8DD-4D77-80EB-3E066FD55168}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{BA500261-FCC6-4C4D-9542-34F3F09F432B}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{96923E9C-BB4B-47C8-9A3C-A7C6B1A96847}"/>
-    <hyperlink ref="F15" r:id="rId6" xr:uid="{782FF733-0012-458C-B7BF-28A0E433F420}"/>
-    <hyperlink ref="F21" r:id="rId7" xr:uid="{19B5DCE6-A05F-4D62-86CA-07D78ADFE698}"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{A178FAE8-B11F-43AB-8C77-7A0C5EC5F6F0}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{390A1AD8-E8DD-4D77-80EB-3E066FD55168}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{BA500261-FCC6-4C4D-9542-34F3F09F432B}"/>
+    <hyperlink ref="F17" r:id="rId4" xr:uid="{782FF733-0012-458C-B7BF-28A0E433F420}"/>
+    <hyperlink ref="F22" r:id="rId5" xr:uid="{19B5DCE6-A05F-4D62-86CA-07D78ADFE698}"/>
+    <hyperlink ref="F21" r:id="rId6" xr:uid="{5B7D99E5-2162-41DA-83AA-F829FC5A69CF}"/>
+    <hyperlink ref="F18" r:id="rId7" xr:uid="{CBF50268-746D-4D90-8A6A-CB74311C00EC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId8"/>
-  <ignoredErrors>
-    <ignoredError sqref="E38 E43" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>